<commit_message>
Added comments to log manager
</commit_message>
<xml_diff>
--- a/Buffer Test Results.xlsx
+++ b/Buffer Test Results.xlsx
@@ -120,14 +120,14 @@
 Block 13 will be replaced because Backward 2 distance of Block 13 is higher than Block 15 and 17 (as it was pinned first during initialization)</t>
   </si>
   <si>
-    <t>Block 13, Block 15 and Block 17 were pinned 3 times (int total) and unpinned 3 times to ensure that the pin count remains zero at the end.
+    <t>1) All the blocks in the buffer pool (except log manager) are pinned once in order 11 to 17
+2) Block 17, Block 15 and Block 13 and pinned 3 times
+3) Block 17, Block 15 and Block 13 are unpinned 4 times
+4) Block 18 and Block 19 will be newly pinned</t>
+  </si>
+  <si>
+    <t>Block 13, Block 15 and Block 17 were pinned 4 times (int total) and unpinned 4 times to ensure that the pin count remains zero at the end.
 Block 15 will be replaced because Backward 2 distance of Block 17 is higher than Block 15 (as the second pin of Block 17 was before Block 15)</t>
-  </si>
-  <si>
-    <t>1) All the blocks in the buffer pool (except log manager) are pinned once in order 11 to 17
-2) Block 17, Block 15 and Block 13 and pinned 2 times
-3) Block 17, Block 15 and Block 13 are unpinned 3 times
-4) Block 18 and Block 19 will be newly pinned</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,13 +628,13 @@
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified log manager testcases
</commit_message>
<xml_diff>
--- a/Buffer Test Results.xlsx
+++ b/Buffer Test Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>S No.</t>
   </si>
@@ -128,6 +128,41 @@
   <si>
     <t>Block 13, Block 15 and Block 17 were pinned 4 times (int total) and unpinned 4 times to ensure that the pin count remains zero at the end.
 Block 15 will be replaced because Backward 2 distance of Block 17 is higher than Block 15 (as the second pin of Block 17 was before Block 15)</t>
+  </si>
+  <si>
+    <t>Output seen</t>
+  </si>
+  <si>
+    <t>In LRU2 Replacement Test 1...
+Event(s):
+Changes in Buffer Pool:
+Buff 4 : Block [file filename, block 13] replaced by Block [file filename, block 18]</t>
+  </si>
+  <si>
+    <t>In LRU2 Replacement Test 2...
+Event(s):
+Changes in Buffer Pool:
+Buff 6 : Block [file filename, block 15] replaced by Block [file filename, block 19]
+Buff 8 : Block [file filename, block 17] replaced by Block [file filename, block 18]</t>
+  </si>
+  <si>
+    <t>In Master LRU test...
+Event(s):
+Changes in Buffer Pool:
+Buff 6 : Block [file filename, block 15] replaced by Block [file filename, block 19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Basic Replacement Test 1...
+Event(s):
+Changes in Buffer Pool:
+Buff 6 : Block [file filename, block 15] replaced by Block [file filename, block 18]
+</t>
+  </si>
+  <si>
+    <t>In Basic Replacement Test 2...
+Event(s):
+Changes in Buffer Pool:
+Buff 4 : Block [file filename, block 13] replaced by Block [file filename, block 18]</t>
   </si>
 </sst>
 </file>
@@ -536,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D693B997-3C26-4151-B975-08B21B3CFAAB}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,10 +584,11 @@
     <col min="3" max="3" width="55.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.5703125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="65.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -568,8 +604,11 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -585,8 +624,11 @@
       <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -602,8 +644,11 @@
       <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -619,8 +664,11 @@
       <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -636,8 +684,11 @@
       <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -652,6 +703,9 @@
       </c>
       <c r="E6" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>